<commit_message>
tengo los 4 tipos de elementos pero no concuerdan las deformaciones
</commit_message>
<xml_diff>
--- a/pruebas_excel/ETABS_modelo/ETABS/revision_2_marco_elemento_a_elemento/datos_prueba2.xlsx
+++ b/pruebas_excel/ETABS_modelo/ETABS/revision_2_marco_elemento_a_elemento/datos_prueba2.xlsx
@@ -8,32 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\ETABS_modelo\ETABS\revision_2_marco_elemento_a_elemento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F630D1-808D-4280-A314-6B99E6AEC710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F9DEFF4-5831-46B2-BC06-75D717D366C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="4740" windowWidth="12000" windowHeight="7995" firstSheet="20" activeTab="20" xr2:uid="{0836F8F1-B425-451E-B716-A39DCD8B1F15}"/>
+    <workbookView xWindow="-30" yWindow="5190" windowWidth="12000" windowHeight="7995" xr2:uid="{7306F667-F0BA-48D9-B4D4-A183920A61C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Beam Object Connectivity" sheetId="1" r:id="rId1"/>
-    <sheet name="Column Object Connectivity" sheetId="2" r:id="rId2"/>
-    <sheet name="Dimension Line Object Geometry" sheetId="3" r:id="rId3"/>
-    <sheet name="Frame Assigns - End Len Offsets" sheetId="4" r:id="rId4"/>
-    <sheet name="Frame Assigns - Frame Auto Mesh" sheetId="5" r:id="rId5"/>
-    <sheet name="Frame Assigns - Insertion Point" sheetId="6" r:id="rId6"/>
-    <sheet name="Frame Assigns - Output Stations" sheetId="7" r:id="rId7"/>
-    <sheet name="Frame Assigns - Sect Prop" sheetId="8" r:id="rId8"/>
-    <sheet name="Frame Assigns - Summary" sheetId="9" r:id="rId9"/>
-    <sheet name="Frame Loads - Open Struct Wind" sheetId="10" r:id="rId10"/>
-    <sheet name="Frame Sec Def - Steel Pipe" sheetId="11" r:id="rId11"/>
-    <sheet name="Frame Prop - Summary" sheetId="12" r:id="rId12"/>
-    <sheet name="Joint Assigns - Restraints" sheetId="13" r:id="rId13"/>
-    <sheet name="Jt Assigns - Summary" sheetId="14" r:id="rId14"/>
-    <sheet name="Joint Loads - Force" sheetId="15" r:id="rId15"/>
-    <sheet name="Mat Prop - Basic Mech Props" sheetId="16" r:id="rId16"/>
-    <sheet name="Point Bays" sheetId="17" r:id="rId17"/>
-    <sheet name="Point Object Connectivity" sheetId="18" r:id="rId18"/>
-    <sheet name="Story Definitions" sheetId="19" r:id="rId19"/>
-    <sheet name="Tower and Base Story Definition" sheetId="20" r:id="rId20"/>
-    <sheet name="Program Control" sheetId="21" r:id="rId21"/>
+    <sheet name="Brace Object Connectivity" sheetId="2" r:id="rId2"/>
+    <sheet name="Column Object Connectivity" sheetId="3" r:id="rId3"/>
+    <sheet name="Dimension Line Object Geometry" sheetId="4" r:id="rId4"/>
+    <sheet name="Frame Assigns - End Len Offsets" sheetId="5" r:id="rId5"/>
+    <sheet name="Frame Assigns - Frame Auto Mesh" sheetId="6" r:id="rId6"/>
+    <sheet name="Frame Assigns - Insertion Point" sheetId="7" r:id="rId7"/>
+    <sheet name="Frame Assigns - Output Stations" sheetId="8" r:id="rId8"/>
+    <sheet name="Frame Assigns - Sect Prop" sheetId="9" r:id="rId9"/>
+    <sheet name="Frame Assigns - Summary" sheetId="10" r:id="rId10"/>
+    <sheet name="Frame Loads - Open Struct Wind" sheetId="11" r:id="rId11"/>
+    <sheet name="Frame Sec Def - Steel Pipe" sheetId="12" r:id="rId12"/>
+    <sheet name="Frame Prop - Summary" sheetId="13" r:id="rId13"/>
+    <sheet name="Joint Assigns - Restraints" sheetId="14" r:id="rId14"/>
+    <sheet name="Jt Assigns - Summary" sheetId="15" r:id="rId15"/>
+    <sheet name="Joint Loads - Force" sheetId="16" r:id="rId16"/>
+    <sheet name="Mat Prop - Basic Mech Props" sheetId="17" r:id="rId17"/>
+    <sheet name="Point Bays" sheetId="18" r:id="rId18"/>
+    <sheet name="Point Object Connectivity" sheetId="19" r:id="rId19"/>
+    <sheet name="Story Definitions" sheetId="20" r:id="rId20"/>
+    <sheet name="Tower and Base Story Definition" sheetId="21" r:id="rId21"/>
+    <sheet name="Program Control" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="227">
   <si>
     <t>TABLE:  Beam Object Connectivity</t>
   </si>
@@ -106,6 +107,18 @@
     <t>d96ec63f-3d23-4a5b-8409-59098e8b6e90</t>
   </si>
   <si>
+    <t>TABLE:  Brace Object Connectivity</t>
+  </si>
+  <si>
+    <t>BraceBay</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>24992240-f2ea-4555-91fd-24f4ba5c22f5</t>
+  </si>
+  <si>
     <t>TABLE:  Column Object Connectivity</t>
   </si>
   <si>
@@ -185,9 +198,6 @@
   </si>
   <si>
     <t>Auto</t>
-  </si>
-  <si>
-    <t>D2</t>
   </si>
   <si>
     <t>TABLE:  Frame Assignments - Frame Auto Mesh Options</t>
@@ -1181,12 +1191,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3C7AFA-390A-4BE3-9E4F-94DC07230E5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521D2A9D-6416-4068-9958-C6CD705C07E3}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:E5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1319,205 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A23057-C86D-4C41-BAD4-80A4D053E9DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87CA483-0489-4AAD-8BE8-5410728D74DE}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C4:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4">
+        <v>5000</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5">
+        <v>5000</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6">
+        <v>7810.25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>6000</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EDA595-748A-440B-9913-BEACD8A51681}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1327,7 +1535,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1340,19 +1548,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,13 +1594,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,19 +1608,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,19 +1628,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1446,13 +1654,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1460,8 +1668,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1495A4-A932-4263-89EA-737DB43BBA0B}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F924B6F-9C3A-479C-AEEF-35A319158EEE}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1487,7 +1695,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1507,52 +1715,52 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1591,13 +1799,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>300</v>
@@ -1630,10 +1838,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1641,8 +1849,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B897734-1088-45EE-A4C0-73AED4F70CF3}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53BF7DE9-EAB6-4348-9218-7E86D575D4A4}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1670,7 +1878,7 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1704,94 +1912,94 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA2" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="AB2" s="11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="AC2" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -1808,40 +2016,40 @@
         <v>8</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>9</v>
@@ -1872,16 +2080,16 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E4">
         <v>11721.3</v>
@@ -1967,12 +2175,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671A5ED7-BEFA-487A-B341-CFC1EE5ACCD5}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37069EC-0B6B-4D1D-9D1B-5C27186B9B7A}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="C4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +2192,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2000,28 +2208,28 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2064,22 +2272,22 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2087,12 +2295,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49834FA-3136-456D-9966-5B2CA60A1C03}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D0E0EDA-BD37-46C7-82AD-0F774FD1E5CB}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C8"/>
+      <selection activeCell="B8" sqref="B4:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2313,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2117,16 +2325,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2157,7 +2365,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2171,7 +2379,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2185,10 +2393,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2202,7 +2410,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2216,7 +2424,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2224,8 +2432,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B6C62A-8482-4506-B364-6FCFE4B6E514}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B336E2-9DD2-4809-918C-04F2F9884397}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2244,7 +2452,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2264,37 +2472,37 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>7</v>
@@ -2314,22 +2522,22 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>9</v>
@@ -2352,7 +2560,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E4">
         <v>5000</v>
@@ -2379,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2393,7 +2601,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E5">
         <v>5000</v>
@@ -2420,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2434,7 +2642,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E6">
         <v>5000</v>
@@ -2461,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2475,7 +2683,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -2502,7 +2710,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2510,8 +2718,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A01902B-76A9-4B67-A7A9-1E6F5FC22CF0}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE784988-4781-4ACE-B479-BD70E15A1055}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2530,7 +2738,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -2542,28 +2750,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,28 +2782,28 @@
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C4">
         <v>2.4000000000000001E-5</v>
@@ -2618,10 +2826,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C5">
         <v>7.7000000000000001E-5</v>
@@ -2638,10 +2846,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C6">
         <v>7.7000000000000001E-5</v>
@@ -2658,10 +2866,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C7">
         <v>7.7000000000000001E-5</v>
@@ -2687,8 +2895,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD346745-8F0A-416D-8889-D8B612D2EC3F}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66B01D2-132B-418F-B4A2-F42CF45BC4B4}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2705,7 +2913,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -2715,19 +2923,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>7</v>
@@ -2758,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2770,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2778,7 +2986,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>6000</v>
@@ -2790,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2798,7 +3006,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>6000</v>
@@ -2810,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,7 +3026,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2830,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2838,12 +3046,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E6DF70-F95B-4A1E-ADD9-32AA10158325}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2615FB2B-1183-49E8-B704-F97172DAC4FE}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="A4:D8"/>
+      <selection activeCell="D4" sqref="A4:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,7 +3066,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2871,28 +3079,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>7</v>
@@ -2932,7 +3140,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -2941,7 +3149,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>6000</v>
@@ -2953,7 +3161,7 @@
         <v>5000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2961,7 +3169,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -2970,7 +3178,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>6000</v>
@@ -2982,7 +3190,7 @@
         <v>5000</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2990,7 +3198,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -2999,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -3011,7 +3219,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3019,7 +3227,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -3028,7 +3236,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>6000</v>
@@ -3040,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3048,7 +3256,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -3057,7 +3265,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -3069,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3077,8 +3285,110 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA74DB4-941E-4FC8-BEB0-08402D99B9FD}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84F3D52-FD81-47D4-9B32-C978CC0B8773}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="13">
+        <v>5</v>
+      </c>
+      <c r="E4" s="13">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>7810.25</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7A3568-6AE6-4587-BAF5-0D8C7553B43B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3098,7 +3408,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
@@ -3109,22 +3419,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>7</v>
@@ -3161,19 +3471,19 @@
         <v>5000</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3181,112 +3491,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A700AE1B-C6A6-4159-8167-BC5D76088DCB}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="13">
-        <v>2</v>
-      </c>
-      <c r="E4" s="13">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>5000</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EC6F72-2B07-4E4E-8E2C-CAAA189815A6}">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0995AB7-E057-4ED9-A7E0-74CB6362D72E}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3305,7 +3511,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3316,25 +3522,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3362,13 +3568,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
@@ -3377,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3385,12 +3591,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEFAD2D-44B5-47D6-A83D-75C10C2AE5AB}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0FF39-5C64-469F-968D-8B3333CA9CD2}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,7 +3617,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3427,40 +3633,40 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3503,40 +3709,40 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3545,7 +3751,111 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A0CBC8-B3A9-467B-9DE6-AB7A0D5EFB39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BBBD03-BE7A-4596-86BF-8D0031881A2D}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="A4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="13">
+        <v>2</v>
+      </c>
+      <c r="E4" s="13">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>5000</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E5A12E-6283-4EB6-A7AF-43769F22714F}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3564,7 +3874,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -3580,34 +3890,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>6</v>
@@ -3656,10 +3966,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3689,7 +3999,7 @@
         <v>6000</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3697,8 +4007,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB865EF-7EFE-4141-8E2E-15D3A3F8909A}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F66A9D9D-6A18-442A-AF10-96A29F0FA477}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3717,7 +4027,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3732,25 +4042,25 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3788,7 +4098,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3800,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3808,13 +4118,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3826,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3834,13 +4144,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -3852,7 +4162,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3866,7 +4176,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -3878,7 +4188,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3886,12 +4196,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B725849B-1C28-4A7E-8FB9-C9E24560D0C1}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E70B7AB-8C87-41B7-8EB5-BAF9021ECA1A}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="C7" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3907,7 +4217,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3922,25 +4232,25 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3980,19 +4290,19 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4000,25 +4310,25 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4026,25 +4336,25 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4058,19 +4368,19 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4078,12 +4388,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5191BC-7254-49E4-9A81-094E655B5A6B}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7616279-1DDA-4218-92DB-0031D495AAFF}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="C7" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,7 +4407,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4111,22 +4421,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4163,16 +4473,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4180,22 +4490,22 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4203,22 +4513,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4232,16 +4542,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -4249,12 +4559,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15389CE1-27CE-4654-81D0-13F8276EF313}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA935A71-62AC-49A7-802C-CD0730F263F5}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="C7" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4268,7 +4578,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4281,19 +4591,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4325,7 +4635,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E4">
         <v>500</v>
@@ -4336,13 +4646,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -4353,13 +4663,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -4376,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E7">
         <v>500</v>
@@ -4387,8 +4697,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD211254-F881-46B6-AF81-896B9DC7157C}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F42FED3-1C35-4C7B-AF38-086C6D697770}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4406,7 +4716,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4419,19 +4729,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4465,13 +4775,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4479,19 +4789,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="13">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4499,19 +4809,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4525,211 +4835,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E150EA54-EA81-4374-9513-4C2956399FA3}">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C4:C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="13">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4">
-        <v>5000</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="13">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5">
-        <v>5000</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="13">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6">
-        <v>7810.25</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7">
-        <v>6000</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7">
-        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
las funciones de dano son correctas, ya coinciden las deformaciones con cargas estaticas aplicadas
</commit_message>
<xml_diff>
--- a/pruebas_excel/ETABS_modelo/ETABS/revision_2_marco_elemento_a_elemento/datos_prueba2.xlsx
+++ b/pruebas_excel/ETABS_modelo/ETABS/revision_2_marco_elemento_a_elemento/datos_prueba2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral_error\pruebas_excel\ETABS_modelo\ETABS\revision_2_marco_elemento_a_elemento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25C22D97-33EA-4861-A691-7DABF987BF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79C20E8C-1791-4263-A06D-EC9B30AB7D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="5115" windowWidth="12000" windowHeight="7995" firstSheet="24" activeTab="24" xr2:uid="{896D9515-79AD-4202-BC02-5A2227C0AAA3}"/>
+    <workbookView xWindow="-30" yWindow="5115" windowWidth="12000" windowHeight="7995" firstSheet="24" activeTab="24" xr2:uid="{6FDDAB84-3AD1-4530-BB01-9E22367FCA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Beam Bays" sheetId="1" r:id="rId1"/>
@@ -383,109 +383,109 @@
     <t>FSec1</t>
   </si>
   <si>
+    <t>FSec2</t>
+  </si>
+  <si>
+    <t>TABLE:  Frame Assignments - Summary</t>
+  </si>
+  <si>
+    <t>Design Type</t>
+  </si>
+  <si>
+    <t>Analysis Section</t>
+  </si>
+  <si>
+    <t>Design Section</t>
+  </si>
+  <si>
+    <t>Max Station Spacing</t>
+  </si>
+  <si>
+    <t>Min Number Stations</t>
+  </si>
+  <si>
+    <t>Beam</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Brace</t>
+  </si>
+  <si>
+    <t>TABLE:  Frame Loads Assignments - Open Structure Wind Parameters</t>
+  </si>
+  <si>
+    <t>Is Loaded</t>
+  </si>
+  <si>
+    <t>Ice Thickness</t>
+  </si>
+  <si>
+    <t>Coefficient Type</t>
+  </si>
+  <si>
+    <t>Program Calculated</t>
+  </si>
+  <si>
+    <t>TABLE:  Frame Section Property Definitions - Steel Pipe</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>From File?</t>
+  </si>
+  <si>
+    <t>Outside Diameter</t>
+  </si>
+  <si>
+    <t>Wall Thickness</t>
+  </si>
+  <si>
+    <t>Area Modifier</t>
+  </si>
+  <si>
+    <t>As2 Modifier</t>
+  </si>
+  <si>
+    <t>As3 Modifier</t>
+  </si>
+  <si>
+    <t>J Modifier</t>
+  </si>
+  <si>
+    <t>I22 Modifier</t>
+  </si>
+  <si>
+    <t>I33 Modifier</t>
+  </si>
+  <si>
+    <t>Mass Modifier</t>
+  </si>
+  <si>
+    <t>Weight Modifier</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>A992Fy50</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>3cba6bfe-ee76-461f-96db-b72fcb0d4e11</t>
+  </si>
+  <si>
     <t>FSec1_corrosion</t>
-  </si>
-  <si>
-    <t>FSec2</t>
-  </si>
-  <si>
-    <t>TABLE:  Frame Assignments - Summary</t>
-  </si>
-  <si>
-    <t>Design Type</t>
-  </si>
-  <si>
-    <t>Analysis Section</t>
-  </si>
-  <si>
-    <t>Design Section</t>
-  </si>
-  <si>
-    <t>Max Station Spacing</t>
-  </si>
-  <si>
-    <t>Min Number Stations</t>
-  </si>
-  <si>
-    <t>Beam</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Brace</t>
-  </si>
-  <si>
-    <t>TABLE:  Frame Loads Assignments - Open Structure Wind Parameters</t>
-  </si>
-  <si>
-    <t>Is Loaded</t>
-  </si>
-  <si>
-    <t>Ice Thickness</t>
-  </si>
-  <si>
-    <t>Coefficient Type</t>
-  </si>
-  <si>
-    <t>Program Calculated</t>
-  </si>
-  <si>
-    <t>TABLE:  Frame Section Property Definitions - Steel Pipe</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>From File?</t>
-  </si>
-  <si>
-    <t>Outside Diameter</t>
-  </si>
-  <si>
-    <t>Wall Thickness</t>
-  </si>
-  <si>
-    <t>Area Modifier</t>
-  </si>
-  <si>
-    <t>As2 Modifier</t>
-  </si>
-  <si>
-    <t>As3 Modifier</t>
-  </si>
-  <si>
-    <t>J Modifier</t>
-  </si>
-  <si>
-    <t>I22 Modifier</t>
-  </si>
-  <si>
-    <t>I33 Modifier</t>
-  </si>
-  <si>
-    <t>Mass Modifier</t>
-  </si>
-  <si>
-    <t>Weight Modifier</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>A992Fy50</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>3cba6bfe-ee76-461f-96db-b72fcb0d4e11</t>
   </si>
   <si>
     <t>Cyan</t>
@@ -1284,7 +1284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7D7165-92BF-4F33-BF97-57457B0A81AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F110E4F-D75B-4E4F-A589-1C7E0E386AD0}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1398,7 +1398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099BABCA-34A8-47C9-B9BC-9AFE3ED2EB05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A403A762-EFEF-49C4-87CA-50AEEE8D8D22}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1753,7 +1753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DD3942-D367-4F07-8933-1F2D6D20E4CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEF8A98-BADA-44FA-BF69-3C94C9F3AB0F}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2027,7 +2027,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF01C47-0CB2-406A-97E5-692196B4EBD4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2FBA30-2235-4C56-82A9-8E3066454FF7}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2170,7 +2170,7 @@
         <v>105</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,7 +2250,7 @@
         <v>105</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2270,7 +2270,7 @@
         <v>105</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>105</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
         <v>105</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
         <v>105</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2339,7 +2339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AA6727-5877-4C80-BEB9-E1BA06F4811B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3108530A-6666-4B26-904C-0D8921E43A4B}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2353,14 +2353,14 @@
     <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2382,22 +2382,22 @@
         <v>74</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4">
         <v>5000</v>
@@ -2464,7 +2464,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5">
         <v>6000</v>
@@ -2490,7 +2490,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6">
         <v>5000</v>
@@ -2516,16 +2516,16 @@
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7">
         <v>6000</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7">
         <v>500</v>
@@ -2542,7 +2542,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -2568,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9">
         <v>5000</v>
@@ -2594,7 +2594,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10">
         <v>5000</v>
@@ -2620,16 +2620,16 @@
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11">
         <v>5000</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I11">
         <v>3</v>
@@ -2646,16 +2646,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12">
         <v>7071.07</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12">
         <v>3</v>
@@ -2672,16 +2672,16 @@
         <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13">
         <v>7810.25</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I13">
         <v>3</v>
@@ -2698,16 +2698,16 @@
         <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14">
         <v>7071.07</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14">
         <v>3</v>
@@ -2724,16 +2724,16 @@
         <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15">
         <v>7810.25</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15">
         <v>3</v>
@@ -2745,7 +2745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A71B06F-ACC2-4169-BF9B-CA11BA092B3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6719FCBA-F02E-4E41-9225-A3188452B691}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2763,7 +2763,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2782,13 +2782,13 @@
         <v>74</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2908,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2988,7 +2988,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3057,7 +3057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6836A5-D403-4DC6-AA05-EE7DE92192FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF550DFA-EA3F-4213-BE34-1ED0642AF621}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3084,7 +3084,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3104,52 +3104,52 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>88</v>
@@ -3227,27 +3227,27 @@
         <v>1</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D5">
-        <v>293.5</v>
+        <v>287</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>6.5</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3282,10 +3282,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>88</v>
@@ -3321,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>144</v>
@@ -3333,7 +3333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F7E686-098A-4835-9020-BC27DEA69F6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E11B169-8362-4492-AF15-099E9554C1BF}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3396,16 +3396,16 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>146</v>
@@ -3462,28 +3462,28 @@
         <v>163</v>
       </c>
       <c r="W2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="AA2" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB2" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AC2" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="AB2" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="AD2" s="11" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -3567,13 +3567,13 @@
         <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4">
         <v>11721.3</v>
@@ -3656,10 +3656,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>104</v>
@@ -3668,46 +3668,46 @@
         <v>142</v>
       </c>
       <c r="E5">
-        <v>11455.8</v>
+        <v>5727.9</v>
       </c>
       <c r="F5">
-        <v>225820656.69999999</v>
+        <v>112728825.2</v>
       </c>
       <c r="G5">
-        <v>112910328.3</v>
+        <v>56364412.600000001</v>
       </c>
       <c r="H5">
-        <v>112910328.3</v>
+        <v>56364412.600000001</v>
       </c>
       <c r="I5">
-        <v>5736.1</v>
+        <v>2865</v>
       </c>
       <c r="J5">
-        <v>5736.1</v>
+        <v>2865</v>
       </c>
       <c r="K5">
-        <v>769406</v>
+        <v>392783.4</v>
       </c>
       <c r="L5">
-        <v>769406</v>
+        <v>392783.4</v>
       </c>
       <c r="M5">
-        <v>769406</v>
+        <v>392783.4</v>
       </c>
       <c r="N5">
-        <v>769406</v>
+        <v>392783.4</v>
       </c>
       <c r="O5">
-        <v>1023575.6</v>
+        <v>511513.2</v>
       </c>
       <c r="P5">
-        <v>1023575.6</v>
+        <v>511513.2</v>
       </c>
       <c r="Q5">
-        <v>99.3</v>
+        <v>99.2</v>
       </c>
       <c r="R5">
-        <v>99.3</v>
+        <v>99.2</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -3748,16 +3748,16 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>104</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6">
         <v>1492.3</v>
@@ -3844,7 +3844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E797CC-08F4-4F9B-BCBE-2694E741E1F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD8AF88-173E-46FA-94C7-30976F7B4A5A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3872,10 +3872,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>168</v>
@@ -3915,7 +3915,7 @@
         <v>171</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>88</v>
@@ -3936,7 +3936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29853FD-342F-4715-A7BC-0DFDD25787CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47064DF-747F-4F5B-8E30-18DE878CE4E2}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4143,7 +4143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4048FA-1A8F-4CE7-8DA3-BF2A39CC6951}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE455FE-B6E0-4E39-94C9-56396CD1B512}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4331,7 +4331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A54A37-5D10-466E-B547-C4A922A115DD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7488E431-8C81-44BA-9938-C62290C93B18}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4504,7 +4504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A0BBA3-D5C5-4484-ADAF-89CE9C5C846A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A369785-2A5A-420A-84E2-71622696267E}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4535,7 +4535,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>187</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>199</v>
@@ -4681,7 +4681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D9ACF8-6DAC-469D-9CC6-DAFE1A70F2A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99528E79-AAB2-4BEA-8A10-6E02FA7E64F8}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4832,11 +4832,11 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CC205C-71F7-49DA-9A96-A306D72A4AA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4788A924-502E-4745-8862-0F4BAB344496}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A4:D11"/>
+      <selection activeCell="A4" sqref="A4:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5158,7 +5158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61581F64-E5C9-4114-AAE6-310CB3D88104}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DB5CA5-E280-479D-91B8-47B27665EE1A}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5189,7 +5189,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>222</v>
@@ -5204,7 +5204,7 @@
         <v>225</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>4</v>
@@ -5250,7 +5250,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>227</v>
@@ -5262,7 +5262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6290D3D9-D960-4924-9A93-786B53F7033C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B796C678-A21F-4127-B819-961FEA0E2E1A}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5295,13 +5295,13 @@
         <v>229</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>230</v>
@@ -5362,7 +5362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE8C9E6-3AB0-45BB-877A-B45BBB7E503D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6509D6-87B2-46AF-9878-63F826812ABE}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -5521,7 +5521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14792F4-EFAF-4A6B-A5B8-83461AC059F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6C31FF-CC41-428C-BD67-EC216E71BA90}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5654,7 +5654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F14F95-9BA5-4B1F-8B89-9AC3A0EC3F28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BE07D7-2BAC-47FF-9515-42211040EA24}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5827,7 +5827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6049BA29-9780-461B-B067-2AE3AD69F9A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DAF054-D898-4803-B8AB-828D81A4F04F}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5960,11 +5960,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC12713-AF79-46CA-8D62-2A28366842F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA248DE-D7A5-41B9-93F1-D5DC0E3A98BB}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="A4:E7"/>
+      <selection activeCell="A4" sqref="A4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6133,7 +6133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6618E7-17E7-4C68-A10E-C8E025D0FF33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D08D36-6DAD-40CA-938B-ABD49990178B}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6286,7 +6286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCB2A95-0D08-4DF7-A051-9D820395A6BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3BE1F5-4E44-46AF-91CF-F45E917EBA66}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6405,7 +6405,7 @@
         <v>80</v>
       </c>
       <c r="E5">
-        <v>146.80000000000001</v>
+        <v>150</v>
       </c>
       <c r="F5">
         <v>150</v>
@@ -6434,7 +6434,7 @@
         <v>150</v>
       </c>
       <c r="F6">
-        <v>146.80000000000001</v>
+        <v>150</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -6683,7 +6683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F45CFD-3B14-46DC-8F09-D054ADD24C3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D8A80D-E5A3-4F08-913C-D3596155C980}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>